<commit_message>
Upload de notícias mais atuais
</commit_message>
<xml_diff>
--- a/principais_noticias.xlsx
+++ b/principais_noticias.xlsx
@@ -456,17 +456,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Seguradoras adotam medidas emergenciais para ajudar litoral de SP</t>
+          <t>Mapfre registra mais de 5.000 acionamentos de assistência no carnaval</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/02/seguradoras-adotam-medidas-emergenciais-para-ajudar-litoral-de-sp/</t>
+          <t>https://www.revistaapolice.com.br/2023/03/mapfre-registra-mais-de-5-000-acionamentos-de-assistencia-no-carnaval/</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Empresas enviam doações e reforçam atendimento para auxiliar atingidos pelos temporais</t>
+          <t>Companhia reforçou atendimento na época para atender alta demanda. Assistências no Litoral Norte representaram 27% do total</t>
         </is>
       </c>
     </row>
@@ -476,17 +476,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>A construção de uma cultura centrada no cliente</t>
+          <t>Bradesco Saúde aprimora experiência do corretor com Inteligência Artificial</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/02/a-construcao-de-uma-cultura-centrada-no-cliente/</t>
+          <t>https://www.revistaapolice.com.br/2023/03/bradesco-saude-aprimora-experiencia-do-corretor-com-inteligencia-artificial/</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Para de fato ter a centralidade no consumidor, faz-se necessário um movimento que extrapole as tendências e ferramentas tecnológicas</t>
+          <t>Disponíveis no Portal de Negócios, novidades agilizam atendimento ao corretor no pós-venda dos produtos SPG</t>
         </is>
       </c>
     </row>
@@ -496,17 +496,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Roubo e furto de motos cresceram 30% e 42%, respectivamente, em São Paulo</t>
+          <t>Allianz fecha parceria com o Rappi para distribuição de seguro via corretor</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/02/roubo-e-furto-de-motos-cresceram-30-e-42-respectivamente-em-sao-paulo/</t>
+          <t>https://www.revistaapolice.com.br/2023/03/allianz-fecha-parceria-com-o-rappi-para-distribuicao-de-seguro-via-corretor/</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Número é 29% maior do que antes da pandemia. Boletim Tracker-Fecap traz as cidades e bairros de São Paulo mais perigosos</t>
+          <t>Ação é voltada é exclusivamente aos clientes Rappi Prime e abrange todas as ofertas e pacotes do seguro Residencial da companhia</t>
         </is>
       </c>
     </row>
@@ -516,17 +516,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Com base nas Leis de Incentivo Fiscal, Europ Assistance apoia projetos sociais</t>
+          <t>Mapfre anuncia Afonso Arinos como head Comercial de Agronegócio</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/02/com-base-nas-leis-de-incentivo-fiscal-europ-assistance-apoia-projetos-sociais/</t>
+          <t>https://www.revistaapolice.com.br/2023/03/mapfre-apresenta-afonso-arinos-como-head-comercial-de-agronegocio/</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>“Hospital do Amor”; “Em busca de uma Estrela” e “Saúde da Mulher” estão entre as iniciativas contempladas pela empresa, além de shows e espetáculos</t>
+          <t>Com 20 anos de experiência em posições de liderança comercial, novo executivo irá liderar estratégias comerciais para a companhia</t>
         </is>
       </c>
     </row>
@@ -536,17 +536,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Iniciada a implementação da Fase II do Open Insurance</t>
+          <t>Akad disponibiliza seguro por assinatura para pequenas e médias empresas</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/02/iniciada-a-implementacao-da-fase-ii-do-open-insurance/</t>
+          <t>https://www.revistaapolice.com.br/2023/03/akad-disponibiliza-seguro-por-assinatura-para-pequenas-e-medias-empresas/</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Com a fase II, inicia-se a possibilidade do compartilhamento, com o devido consentimento, de dados pessoais de clientes</t>
+          <t>Parceria com a MarketUP e a PDV Box é aposta da seguradora para chegar a mais de 150 mil usuários ativos</t>
         </is>
       </c>
     </row>
@@ -556,17 +556,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Brasilseg cresce 30,7% em prêmios emitidos em 2022</t>
+          <t>Tokio Marine registra crescimento de 40,6% na produção em 2022</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/02/brasilseg-cresce-307-em-premios-emitidos-em-2022/</t>
+          <t>https://www.revistaapolice.com.br/2023/03/tokio-marine-registra-crescimento-de-406-na-producao-em-2022/</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Número corresponde a R$ 15,77 bilhões arrecadados. Seguro Rural, Prestamista e Empresarial se destacam na composição do resultado</t>
+          <t>A produção da companhia atingiu a marca de R$ 10,6 bilhões em faturamento, meta inicialmente prevista para ser alcançada apenas em 2024</t>
         </is>
       </c>
     </row>
@@ -576,17 +576,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>MetLife realiza premiação para as assessorias de investimentos parceiras</t>
+          <t>PDMS quer levar seguro para fatia maior da população</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/02/metlife-realiza-premiacao-para-as-assessorias-de-investimentos-parceiras/</t>
+          <t>https://www.revistaapolice.com.br/2023/03/pdms-quer-levar-seguro-para-fatia-maior-da-populacao/</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Os 70 ganhadores da campanha Get It 2022 foram premiados com uma viagem para Nova Iorque, onde poderão conhecer a sede da seguradora</t>
+          <t>Plano de Desenvolvimento do Mercado de Seguros possui 65 diretrizes em 4 áreas para aumentar o nível de proteção do País</t>
         </is>
       </c>
     </row>
@@ -596,17 +596,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Plano de saúde mais barato é principal razão para portabilidade de carências</t>
+          <t>Mapfre patrocina musical sobre a história do grupo Los Hermanos</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/02/plano-de-saude-mais-barato-e-principal-razao-para-portabilidade-de-carencias/</t>
+          <t>https://www.revistaapolice.com.br/2023/03/mapfre-patrocina-musical-sobre-a-historia-do-grupo-los-hermanos/</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>De acordo com dados divulgados pela ANS, foram mais de 300 mil consultas ao exercício da portabilidade de carências ao longo de 2022</t>
+          <t>Espetáculo, que tem a direção de Michel Melamed, estreia nesta sexta-feira, dia 17 de março, no Teatro Casa Grande, no Rio de Janeiro</t>
         </is>
       </c>
     </row>
@@ -616,17 +616,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Suhai dá 7 dicas para cuidados em enchentes</t>
+          <t>SulAmérica lança linha de produtos Odonto Individual</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/02/suhai-da-7-dicas-para-cuidados-em-enchentes/</t>
+          <t>https://www.revistaapolice.com.br/2023/03/sulamerica-lanca-linha-de-produtos-odonto-individual/</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Objetivo da seguradora é disseminar informações para garantir a segurança dos motoristas e a conservação dos veículos</t>
+          <t>Desconto progressivo para dependentes e elegibilidade para toda a família estão entre os novos benefícios nos planos odontológicos da companhia</t>
         </is>
       </c>
     </row>
@@ -636,17 +636,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Arbitralis digitaliza e acelera processos de arbitragem</t>
+          <t>Generali apresenta resultado operacional de 6,5 bi de euros em 2022</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/02/arbitralis-digitaliza-e-acelera-processos-de-arbitragem/</t>
+          <t>https://www.revistaapolice.com.br/2023/03/generali-apresenta-resultado-operacional-de-65-bi-de-euros-em-2022/</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Lawtech Arbitralis digitalizou totalmente o processo de demandas para a Câmara Brasileira de Arbitragem, democratizando o acesso à justiça</t>
+          <t>De acordo com a companhia, o resultado operacional cresceu devido à expansão do segmento Vida, juntamente com Property and Casualty</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update files to newest news
</commit_message>
<xml_diff>
--- a/principais_noticias.xlsx
+++ b/principais_noticias.xlsx
@@ -476,17 +476,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Bradesco Saúde aprimora experiência do corretor com Inteligência Artificial</t>
+          <t>Allianz fecha parceria com o Rappi para distribuição de seguro via corretor</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/03/bradesco-saude-aprimora-experiencia-do-corretor-com-inteligencia-artificial/</t>
+          <t>https://www.revistaapolice.com.br/2023/03/allianz-fecha-parceria-com-o-rappi-para-distribuicao-de-seguro-via-corretor/</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Disponíveis no Portal de Negócios, novidades agilizam atendimento ao corretor no pós-venda dos produtos SPG</t>
+          <t>Ação é voltada é exclusivamente aos clientes Rappi Prime e abrange todas as ofertas e pacotes do seguro Residencial da companhia</t>
         </is>
       </c>
     </row>
@@ -496,17 +496,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Allianz fecha parceria com o Rappi para distribuição de seguro via corretor</t>
+          <t>Mapfre anuncia Afonso Arinos como head Comercial de Agronegócio</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/03/allianz-fecha-parceria-com-o-rappi-para-distribuicao-de-seguro-via-corretor/</t>
+          <t>https://www.revistaapolice.com.br/2023/03/mapfre-apresenta-afonso-arinos-como-head-comercial-de-agronegocio/</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Ação é voltada é exclusivamente aos clientes Rappi Prime e abrange todas as ofertas e pacotes do seguro Residencial da companhia</t>
+          <t>Com 20 anos de experiência em posições de liderança comercial, novo executivo irá liderar estratégias comerciais para a companhia</t>
         </is>
       </c>
     </row>
@@ -516,17 +516,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Mapfre anuncia Afonso Arinos como head Comercial de Agronegócio</t>
+          <t>Brasilprev lança iniciativa de capacitação exclusiva para PCD’s</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/03/mapfre-apresenta-afonso-arinos-como-head-comercial-de-agronegocio/</t>
+          <t>https://www.revistaapolice.com.br/2023/03/brasilprev-lanca-iniciativa-de-capacitacao-exclusiva-para-pcds/</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Com 20 anos de experiência em posições de liderança comercial, novo executivo irá liderar estratégias comerciais para a companhia</t>
+          <t>Com o objetivo de atrair, capacitar e contratar pessoas com deficiência, programa Lado a Lado irá treinar 50 profissionais em Tecnologia</t>
         </is>
       </c>
     </row>
@@ -536,17 +536,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Akad disponibiliza seguro por assinatura para pequenas e médias empresas</t>
+          <t>Metaverso em seguros: Uma realidade distante?</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/03/akad-disponibiliza-seguro-por-assinatura-para-pequenas-e-medias-empresas/</t>
+          <t>https://www.revistaapolice.com.br/2023/03/metaverso-em-seguros-uma-realidade-distante/</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Parceria com a MarketUP e a PDV Box é aposta da seguradora para chegar a mais de 150 mil usuários ativos</t>
+          <t>O Metaverso oferece um potencial significativo ao setor, atuando, por exemplo, como uma nova abordagem para alcançar o público mais jovem</t>
         </is>
       </c>
     </row>
@@ -556,17 +556,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Tokio Marine registra crescimento de 40,6% na produção em 2022</t>
+          <t>Aumento de desastres naturais reforçam importância do seguro residencial</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/03/tokio-marine-registra-crescimento-de-406-na-producao-em-2022/</t>
+          <t>https://www.revistaapolice.com.br/2023/03/aumento-de-desastres-naturais-reforcam-importancia-do-seguro-residencial/</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>A produção da companhia atingiu a marca de R$ 10,6 bilhões em faturamento, meta inicialmente prevista para ser alcançada apenas em 2024</t>
+          <t>Segundo dados da FenaSeg, apenas 15% das residências brasileiras que contam com um seguro residencial possuem cobertura contra enchentes</t>
         </is>
       </c>
     </row>
@@ -576,17 +576,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>PDMS quer levar seguro para fatia maior da população</t>
+          <t>Akad disponibiliza seguro por assinatura para pequenas e médias empresas</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/03/pdms-quer-levar-seguro-para-fatia-maior-da-populacao/</t>
+          <t>https://www.revistaapolice.com.br/2023/03/akad-disponibiliza-seguro-por-assinatura-para-pequenas-e-medias-empresas/</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Plano de Desenvolvimento do Mercado de Seguros possui 65 diretrizes em 4 áreas para aumentar o nível de proteção do País</t>
+          <t>Parceria com a MarketUP e a PDV Box é aposta da seguradora para chegar a mais de 150 mil usuários ativos</t>
         </is>
       </c>
     </row>
@@ -596,17 +596,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Mapfre patrocina musical sobre a história do grupo Los Hermanos</t>
+          <t>Tokio Marine registra crescimento de 40,6% na produção em 2022</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/03/mapfre-patrocina-musical-sobre-a-historia-do-grupo-los-hermanos/</t>
+          <t>https://www.revistaapolice.com.br/2023/03/tokio-marine-registra-crescimento-de-406-na-producao-em-2022/</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Espetáculo, que tem a direção de Michel Melamed, estreia nesta sexta-feira, dia 17 de março, no Teatro Casa Grande, no Rio de Janeiro</t>
+          <t>A produção da companhia atingiu a marca de R$ 10,6 bilhões em faturamento, meta inicialmente prevista para ser alcançada apenas em 2024</t>
         </is>
       </c>
     </row>
@@ -616,17 +616,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>SulAmérica lança linha de produtos Odonto Individual</t>
+          <t>PDMS quer levar seguro para fatia maior da população</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/03/sulamerica-lanca-linha-de-produtos-odonto-individual/</t>
+          <t>https://www.revistaapolice.com.br/2023/03/pdms-quer-levar-seguro-para-fatia-maior-da-populacao/</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Desconto progressivo para dependentes e elegibilidade para toda a família estão entre os novos benefícios nos planos odontológicos da companhia</t>
+          <t>Plano de Desenvolvimento do Mercado de Seguros possui 65 diretrizes em 4 áreas para aumentar o nível de proteção do País</t>
         </is>
       </c>
     </row>
@@ -636,17 +636,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Generali apresenta resultado operacional de 6,5 bi de euros em 2022</t>
+          <t>Mapfre patrocina musical sobre a história do grupo Los Hermanos</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/03/generali-apresenta-resultado-operacional-de-65-bi-de-euros-em-2022/</t>
+          <t>https://www.revistaapolice.com.br/2023/03/mapfre-patrocina-musical-sobre-a-historia-do-grupo-los-hermanos/</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>De acordo com a companhia, o resultado operacional cresceu devido à expansão do segmento Vida, juntamente com Property and Casualty</t>
+          <t>Espetáculo, que tem a direção de Michel Melamed, estreia nesta sexta-feira, dia 17 de março, no Teatro Casa Grande, no Rio de Janeiro</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update files to the newest news
</commit_message>
<xml_diff>
--- a/principais_noticias.xlsx
+++ b/principais_noticias.xlsx
@@ -456,17 +456,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ameaças cibernéticas e lucros cessantes continuam entre principais riscos empresariais no mundo</t>
+          <t>Alessandro Octaviani toma posse como superintendente da Susep</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/03/ameacas-ciberneticas-e-lucros-cessantes-continuam-entre-principais-riscos-empresariais-no-mundo/</t>
+          <t>https://www.revistaapolice.com.br/2023/04/alessandro-octaviani-toma-posse-como-superintendente-da-susep/</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Segundo um relatório da AGCS, catástrofes naturais e a mudança climática caem no ranking à medida que as empresas priorizam as preocupações macroeconômicas urgentes</t>
+          <t>O novo superintendente entrará em exercício na próxima segunda-feira, 10 de abril, dedicando a primeira semana a reuniões e despachos internos, para apresentação dos projetos em curso na autarquia</t>
         </is>
       </c>
     </row>
@@ -476,17 +476,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Crescimento de roubo e furto de veículos reforça importância do seguro automóvel</t>
+          <t>Marcelo Blay e Manes Erlichman assumem nova posição na Creditas</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/04/crescimento-de-roubo-e-furto-de-veiculos-reforca-importancia-do-seguro-automovel/</t>
+          <t>https://www.revistaapolice.com.br/2023/04/marcelo-blay-e-manes-erlichman-assumem-nova-posicao-na-creditas/</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>De acordo com dados do IBGE, o Brasil registrou cerca de 64 roubos e furtos de veículos por hora em 2022</t>
+          <t>Marcelo Blay e Manes Erlichman assumem a posição de senior advisors na Creditas, que adquiriu a Minuto Seguros em julho de 2021</t>
         </is>
       </c>
     </row>
@@ -516,17 +516,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Marcelo Blay e Manes Erlichman assumem nova posição na Creditas</t>
+          <t>Crescimento de roubo e furto de veículos reforça importância do seguro automóvel</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/04/marcelo-blay-e-manes-erlichman-assumem-nova-posicao-na-creditas/</t>
+          <t>https://www.revistaapolice.com.br/2023/04/crescimento-de-roubo-e-furto-de-veiculos-reforca-importancia-do-seguro-automovel/</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Marcelo Blay e Manes Erlichman assumem a posição de senior advisors na Creditas, que adquiriu a Minuto Seguros em julho de 2021</t>
+          <t>De acordo com dados do IBGE, o Brasil registrou cerca de 64 roubos e furtos de veículos por hora em 2022</t>
         </is>
       </c>
     </row>
@@ -536,17 +536,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Alessandro Octaviani toma posse como superintendente da Susep</t>
+          <t>Susep participa de painéis na Oficina FIDES</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/04/alessandro-octaviani-toma-posse-como-superintendente-da-susep/</t>
+          <t>https://www.revistaapolice.com.br/2023/04/susep-participa-de-paineis-na-oficina-fides/</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>O novo superintendente entrará em exercício na próxima segunda-feira, 10 de abril, dedicando a primeira semana a reuniões e despachos internos, para apresentação dos projetos em curso na autarquia</t>
+          <t>Evento é realizado pela CNseg nos dias 13 e 14 de abril, em Brasília, abordando os temas Sustentabilidade e Riscos Cibernéticos</t>
         </is>
       </c>
     </row>
@@ -556,17 +556,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Mercado de seguros aproveita crescimento da indústria pet para ofertar produtos</t>
+          <t>Seguros SURA registra crescimento em Minas Gerais e no Centro-Oeste</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/04/mercado-de-seguros-aproveita-crescimento-da-industria-pet-para-ofertar-produtos/</t>
+          <t>https://www.revistaapolice.com.br/2023/04/seguros-sura-registra-crescimento-em-minas-gerais-e-no-centro-oeste/</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Levantamento do Instituto Pet Brasil prevê que o segmento fechou 2022 com um faturamento de R$ 59,9 bilhões</t>
+          <t>Objetivo da seguradora é continuar desenvolvendo produtos para ampliar sua carteira de clientes nas regiões</t>
         </is>
       </c>
     </row>
@@ -576,17 +576,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Encontro do CCS-SP discute retorno do corretor ao Open Insurance</t>
+          <t>Seguros Unimed investe em data lakehouse com tecnologia da AWS</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/04/encontro-do-ccs-sp-discute-retorno-do-corretor-de-seguros-ao-open-insurance/</t>
+          <t>https://www.revistaapolice.com.br/2023/04/seguros-unimed-investe-em-data-lakehouse-com-tecnologia-da-aws/</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Ex-diretor e ex-superintendente da Susep explicam aos associados detalhes da resolução que extinguiu a SISS e criou a SPOC</t>
+          <t>Objetivo principal da seguradora é ser uma empresa data driven, garantindo o cumprimento das normas da LGPD</t>
         </is>
       </c>
     </row>
@@ -596,17 +596,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>GBOEX aposta em novo conceito de comunicação</t>
+          <t>Bradesco Vida e Previdência lança ‘Pensão Temporária Bradesco’</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/04/gboex-aposta-em-novo-conceito-de-comunicacao/</t>
+          <t>https://www.revistaapolice.com.br/2023/04/bradesco-vida-e-previdencia-lanca-pensao-temporaria-bradesco/</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Empresa revisitou linha de comunicação e procurou atualizar projetos para traduzirem as alterações e inovações em sua gestão</t>
+          <t>Novo produto oferece flexibilidade na escolha de beneficiários, pensão por até 20 anos e pecúlio para uso imediato em caso da falta do contratante</t>
         </is>
       </c>
     </row>
@@ -616,17 +616,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Gestão financeira deve ser prioridade para pequenos empresários</t>
+          <t>Open Insurance: Segunda fase gera grande expectativas para insurtechs</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/04/gestao-financeira-deve-ser-prioridade-para-pequenos-empresarios/</t>
+          <t>https://www.revistaapolice.com.br/2023/04/open-insurance-segunda-fase-gera-grande-expectativas-para-insurtechs/</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Empreendedores devem apostar em organizar sua forma de controlar os gastos, lucros, investimentos e priorizar o uso da conta de banco jurídica</t>
+          <t>Startups do setor de seguros têm mais facilidade para aderir ao novo sistema e explorar oportunidades com decisões baseadas em dados</t>
         </is>
       </c>
     </row>
@@ -636,17 +636,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SulAmérica reforça linha Odonto PME e Empresarial</t>
+          <t>Aumento de roubo de celulares reforça importância do seguro</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://www.revistaapolice.com.br/2023/04/sulamerica-reforca-linha-odonto-pme-e-empresarial/</t>
+          <t>https://www.revistaapolice.com.br/2023/04/aumento-de-roubo-de-celulares-reforca-importancia-do-seguro/</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Após anunciar novidades no portfólio Odonto Individual, companhia apresenta lançamentos e novos benefícios para os planos PME, PME Mais e Empresarial</t>
+          <t>Somente em São Paulo, mais de duzentos mil celulares foram roubados em 2022 segundo dados da Secretária de Segurança Pública</t>
         </is>
       </c>
     </row>

</xml_diff>